<commit_message>
modify data driven login test
</commit_message>
<xml_diff>
--- a/Test Data/LoginData.xlsx
+++ b/Test Data/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!MY FOLDER\QA Testing\Automation Projects\Petrovue\IDM\IDM\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354E82B8-274C-41F8-8352-67C9A88F3A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6A7401-38E5-4F34-86CD-A568B76D5E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1470" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -45,12 +45,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>petrolink123</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>8SQVv/p9jVRYfSV/eMGvjg==</t>
   </si>
   <si>
@@ -63,13 +57,19 @@
     <t>P9ET2sDE0SE=</t>
   </si>
   <si>
-    <t>tzH6RvlfSTg=</t>
-  </si>
-  <si>
-    <t>ZOCG6GzvUJdzK5VZBdysRw==</t>
-  </si>
-  <si>
-    <t>J7R4ejOak4Y=</t>
+    <t>Password1</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>administrator</t>
   </si>
 </sst>
 </file>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +400,7 @@
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,73 +408,80 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>123</v>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>